<commit_message>
developed coke oven unit
</commit_message>
<xml_diff>
--- a/data/fuels.xlsx
+++ b/data/fuels.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/demoData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7BB493-5971-B14A-AAFD-0B7637EF40E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="27640" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="1065" windowWidth="27645" windowHeight="16005"/>
   </bookViews>
   <sheets>
     <sheet name="Fuels" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="fuels" localSheetId="0">Fuels!$A$1:$D$7</definedName>
+    <definedName name="fuels" localSheetId="0">Fuels!$A$1:$E$7</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="fuels" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="fuels" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="/Users/Tanzer/GitHub/BlackBlox/globalData/fuels.tsv" thousands=" ">
       <textFields count="4">
         <textField/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>meta-notes</t>
   </si>
@@ -86,12 +85,54 @@
   </si>
   <si>
     <t>Eurofer electricity mix proxy</t>
+  </si>
+  <si>
+    <t>meta-source</t>
+  </si>
+  <si>
+    <t>EUROFER</t>
+  </si>
+  <si>
+    <t>Moisture Content</t>
+  </si>
+  <si>
+    <t>t / t wet</t>
+  </si>
+  <si>
+    <t>coking coal</t>
+  </si>
+  <si>
+    <t>IEAGHG 2013</t>
+  </si>
+  <si>
+    <t>LHV</t>
+  </si>
+  <si>
+    <t>(gj/t dry)</t>
+  </si>
+  <si>
+    <t>C content</t>
+  </si>
+  <si>
+    <t>H content</t>
+  </si>
+  <si>
+    <t>S content</t>
+  </si>
+  <si>
+    <t>Ash content</t>
+  </si>
+  <si>
+    <t>PCI coal</t>
+  </si>
+  <si>
+    <t>IEAGHG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -630,7 +671,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="fuels" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="fuels" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -929,22 +970,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.125" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -952,16 +995,37 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>0</v>
       </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -969,125 +1033,238 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>33.700000000000003</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <f>3.19</f>
         <v>3.19</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>29.6</v>
       </c>
       <c r="C4">
+        <v>28.4</v>
+      </c>
+      <c r="D4">
+        <f>2.93</f>
         <v>2.93</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C5">
+        <v>47</v>
+      </c>
+      <c r="D5">
         <v>2.75</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
-        <v>45.3</v>
+        <v>45.6</v>
       </c>
       <c r="C6">
+        <v>38.6</v>
+      </c>
+      <c r="D6">
         <v>3.15</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
-        <v>21</v>
+        <v>16.2</v>
       </c>
       <c r="C7">
+        <v>15.4</v>
+      </c>
+      <c r="D7">
         <v>1.8</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
         <v>2.77</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.11</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B10">
+        <v>29</v>
+      </c>
+      <c r="C10">
         <v>29.01</v>
       </c>
-      <c r="C9">
+      <c r="D10">
         <v>3.23</v>
       </c>
-      <c r="D9">
+      <c r="F10">
+        <v>0.04</v>
+      </c>
+      <c r="G10">
+        <v>0.88049999999999995</v>
+      </c>
+      <c r="H10">
+        <v>1E-3</v>
+      </c>
+      <c r="I10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J10">
+        <f>1-SUM(G10:I10)</f>
+        <v>0.11250000000000004</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>32.6</v>
+      </c>
+      <c r="C11">
+        <v>31.1</v>
+      </c>
+      <c r="D11">
+        <v>3.19</v>
+      </c>
+      <c r="E11">
         <v>0</v>
       </c>
+      <c r="F11">
+        <v>0.08</v>
+      </c>
+      <c r="G11">
+        <v>0.78849999999999998</v>
+      </c>
+      <c r="H11">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f>1-SUM(G11:I11)</f>
+        <v>0.16639999999999999</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0.11</v>
-      </c>
-      <c r="D10">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>22.27</v>
+      </c>
+      <c r="D12">
+        <f>D10</f>
+        <v>3.23</v>
+      </c>
+      <c r="F12">
+        <v>0.01</v>
+      </c>
+      <c r="G12">
+        <v>0.87</v>
+      </c>
+      <c r="H12">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="I12">
         <v>0</v>
+      </c>
+      <c r="J12">
+        <f>1-SUM(G12:I12)</f>
+        <v>8.9700000000000002E-2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added data for sinter plant and blast furnace
</commit_message>
<xml_diff>
--- a/data/fuels.xlsx
+++ b/data/fuels.xlsx
@@ -974,7 +974,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1173,6 +1173,9 @@
       <c r="D10">
         <v>3.23</v>
       </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
       <c r="F10">
         <v>0.04</v>
       </c>
@@ -1242,6 +1245,9 @@
       <c r="D12">
         <f>D10</f>
         <v>3.23</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0.01</v>

</xml_diff>